<commit_message>
Assignmnet completed only comment need to add
</commit_message>
<xml_diff>
--- a/MainAssignment/DataFile/Barrow_book_details.xlsx
+++ b/MainAssignment/DataFile/Barrow_book_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mumarkhan\eclipse-workspace\PIPAssignment\MainAssignment\DataFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A24B784-2B1B-46C3-A128-9692A5853870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6FB633-E5D0-4246-9493-331DBF48D98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3150" yWindow="2260" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -31,16 +31,28 @@
     <t>Isbn</t>
   </si>
   <si>
-    <t>umarkhan</t>
-  </si>
-  <si>
-    <t>Hacking</t>
-  </si>
-  <si>
-    <t>1234567890</t>
-  </si>
-  <si>
-    <t>armanalam</t>
+    <t>umarkhan1</t>
+  </si>
+  <si>
+    <t>java_book</t>
+  </si>
+  <si>
+    <t>0987654321-z</t>
+  </si>
+  <si>
+    <t>c++</t>
+  </si>
+  <si>
+    <t>543211234-z</t>
+  </si>
+  <si>
+    <t>farman</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>12345678901</t>
   </si>
 </sst>
 </file>
@@ -396,7 +408,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -428,36 +440,19 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>